<commit_message>
Clean 2015 and 2014 tower data. Puffin problem still exists
</commit_message>
<xml_diff>
--- a/data/tower_count/tower_count_2015.xlsx
+++ b/data/tower_count/tower_count_2015.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejgna\Documents\project-eleanor-and-wriley\data\tower_count\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86406D83-006A-41D7-B310-8EB34AC60F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="7935"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -189,6 +195,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -237,7 +246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,9 +279,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,6 +331,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -480,11 +523,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +557,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42530</v>
+        <v>42164</v>
       </c>
       <c r="B2">
         <v>448</v>
@@ -537,7 +580,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42531</v>
+        <v>42165</v>
       </c>
       <c r="B3">
         <v>465</v>
@@ -560,7 +603,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41801</v>
+        <v>42166</v>
       </c>
       <c r="B4">
         <v>359</v>
@@ -583,7 +626,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41802</v>
+        <v>42167</v>
       </c>
       <c r="B5">
         <v>409</v>
@@ -606,7 +649,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41803</v>
+        <v>42168</v>
       </c>
       <c r="B6">
         <v>371</v>
@@ -629,7 +672,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41804</v>
+        <v>42169</v>
       </c>
       <c r="B7">
         <v>342</v>
@@ -652,7 +695,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41805</v>
+        <v>42170</v>
       </c>
       <c r="B8">
         <v>460</v>
@@ -675,7 +718,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41806</v>
+        <v>42171</v>
       </c>
       <c r="B9">
         <v>422</v>
@@ -698,7 +741,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41807</v>
+        <v>42172</v>
       </c>
       <c r="B10">
         <v>402</v>
@@ -721,7 +764,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41808</v>
+        <v>42173</v>
       </c>
       <c r="B11">
         <v>455</v>
@@ -744,7 +787,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41809</v>
+        <v>42174</v>
       </c>
       <c r="B12">
         <v>379</v>
@@ -767,7 +810,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41810</v>
+        <v>42175</v>
       </c>
       <c r="B13">
         <v>484</v>
@@ -790,7 +833,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41811</v>
+        <v>42176</v>
       </c>
       <c r="B14">
         <v>436</v>
@@ -813,7 +856,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41812</v>
+        <v>42177</v>
       </c>
       <c r="B15">
         <v>546</v>
@@ -836,7 +879,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41813</v>
+        <v>42178</v>
       </c>
       <c r="B16">
         <v>556</v>
@@ -859,7 +902,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41814</v>
+        <v>42179</v>
       </c>
       <c r="B17">
         <v>567</v>
@@ -879,7 +922,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41815</v>
+        <v>42180</v>
       </c>
       <c r="B18">
         <v>507</v>
@@ -899,7 +942,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41816</v>
+        <v>42181</v>
       </c>
       <c r="B19">
         <v>534</v>
@@ -922,7 +965,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41817</v>
+        <v>42182</v>
       </c>
       <c r="B20">
         <v>536</v>
@@ -945,12 +988,12 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41818</v>
+        <v>42183</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41819</v>
+        <v>42184</v>
       </c>
       <c r="B22">
         <v>507</v>
@@ -973,12 +1016,12 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41820</v>
+        <v>42185</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41821</v>
+        <v>42186</v>
       </c>
       <c r="B24">
         <v>587</v>
@@ -1001,7 +1044,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41822</v>
+        <v>42187</v>
       </c>
       <c r="B25">
         <v>428</v>
@@ -1024,7 +1067,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41823</v>
+        <v>42188</v>
       </c>
       <c r="B26">
         <v>448</v>
@@ -1047,17 +1090,17 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41824</v>
+        <v>42189</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41825</v>
+        <v>42190</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41826</v>
+        <v>42191</v>
       </c>
       <c r="B29">
         <v>502</v>
@@ -1080,7 +1123,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41827</v>
+        <v>42192</v>
       </c>
       <c r="B30">
         <v>577</v>
@@ -1103,12 +1146,12 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41828</v>
+        <v>42193</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41829</v>
+        <v>42194</v>
       </c>
       <c r="B32">
         <v>632</v>
@@ -1131,7 +1174,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>41830</v>
+        <v>42195</v>
       </c>
       <c r="B33">
         <v>558</v>
@@ -1154,7 +1197,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>41831</v>
+        <v>42196</v>
       </c>
       <c r="B34">
         <v>563</v>
@@ -1177,7 +1220,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>41832</v>
+        <v>42197</v>
       </c>
       <c r="B35">
         <v>519</v>
@@ -1200,7 +1243,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>41833</v>
+        <v>42198</v>
       </c>
       <c r="B36">
         <v>526</v>
@@ -1223,17 +1266,17 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>41834</v>
+        <v>42199</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>41835</v>
+        <v>42200</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41836</v>
+        <v>42201</v>
       </c>
       <c r="B39">
         <v>463</v>
@@ -1256,7 +1299,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41837</v>
+        <v>42202</v>
       </c>
       <c r="B40">
         <v>472</v>
@@ -1279,7 +1322,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>41838</v>
+        <v>42203</v>
       </c>
       <c r="B41">
         <v>496</v>
@@ -1299,22 +1342,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41839</v>
+        <v>42204</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41840</v>
+        <v>42205</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>41841</v>
+        <v>42206</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>41842</v>
+        <v>42207</v>
       </c>
       <c r="B45">
         <v>480</v>
@@ -1328,7 +1371,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>41843</v>
+        <v>42208</v>
       </c>
       <c r="B46">
         <v>519</v>
@@ -1351,7 +1394,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>41844</v>
+        <v>42209</v>
       </c>
       <c r="B47">
         <v>524</v>
@@ -1374,7 +1417,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>41845</v>
+        <v>42210</v>
       </c>
       <c r="B48">
         <v>564</v>
@@ -1397,7 +1440,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>41846</v>
+        <v>42211</v>
       </c>
       <c r="B49">
         <v>581</v>
@@ -1420,17 +1463,17 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>41847</v>
+        <v>42212</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>41848</v>
+        <v>42213</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>41849</v>
+        <v>42214</v>
       </c>
       <c r="B52">
         <v>507</v>
@@ -1450,7 +1493,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>42593</v>
+        <v>42227</v>
       </c>
       <c r="B53">
         <v>428</v>
@@ -1477,7 +1520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1489,7 +1532,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>